<commit_message>
Updated table of times for Lab2_1
</commit_message>
<xml_diff>
--- a/Lab2/Lab2_times.xlsx
+++ b/Lab2/Lab2_times.xlsx
@@ -34,10 +34,10 @@
     <t>0.687562</t>
   </si>
   <si>
-    <t>0.677354</t>
-  </si>
-  <si>
-    <t>0.743037</t>
+    <t>2.56307</t>
+  </si>
+  <si>
+    <t>4.33656</t>
   </si>
   <si>
     <t>8 threads</t>
@@ -49,10 +49,10 @@
     <t>0.65105</t>
   </si>
   <si>
-    <t>0.563635</t>
-  </si>
-  <si>
-    <t>0.678584</t>
+    <t xml:space="preserve"> 3.36031</t>
+  </si>
+  <si>
+    <t>4.38572</t>
   </si>
   <si>
     <t>16 threads</t>
@@ -64,10 +64,10 @@
     <t>0.643949</t>
   </si>
   <si>
-    <t>0.537653</t>
-  </si>
-  <si>
-    <t>0.69607</t>
+    <t>5.78905</t>
+  </si>
+  <si>
+    <t>4.18408</t>
   </si>
   <si>
     <t>32 threads</t>
@@ -79,10 +79,10 @@
     <t>0.635394</t>
   </si>
   <si>
-    <t>0.555062</t>
-  </si>
-  <si>
-    <t>0.803642</t>
+    <t>6.01106</t>
+  </si>
+  <si>
+    <t>3.15639</t>
   </si>
 </sst>
 </file>
@@ -387,10 +387,10 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -407,10 +407,10 @@
       <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -427,10 +427,10 @@
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -447,10 +447,10 @@
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>